<commit_message>
Change name of a few colums
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisf\Dropbox\2_WORK\EperLab\Proyectos\2020_FiscalImpactDecarbonization\4_Model\WORKING_MODEL_FRAMEWORK_July2020\Scenario_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D9B31D-B988-459A-B096-2473F6127B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E27D937-B741-4E65-9CDC-EAE53815D596}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="-13980" windowWidth="17940" windowHeight="12360" tabRatio="864" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -190,9 +190,6 @@
     <t>TRYLF</t>
   </si>
   <si>
-    <t>Plain_English</t>
-  </si>
-  <si>
     <t>Electric</t>
   </si>
   <si>
@@ -359,6 +356,9 @@
   </si>
   <si>
     <t>Tren de Carga</t>
+  </si>
+  <si>
+    <t>Plain English</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -874,12 +874,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -910,17 +908,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,7 +923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -943,7 +936,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1250,14 +1242,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>17</v>
@@ -1267,112 +1259,112 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15"/>
+      <c r="A2" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+        <v>83</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="18"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="18"/>
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="18"/>
+      <c r="B6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="18"/>
+      <c r="B7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
+      <c r="B8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="18"/>
+        <v>89</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="16"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1388,7 +1380,7 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1409,13 +1401,13 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>4</v>
@@ -1433,7 +1425,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>1</v>
@@ -1446,28 +1438,28 @@
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="34" t="s">
+      <c r="B2" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="27" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1475,24 +1467,24 @@
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="18" t="s">
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1500,24 +1492,24 @@
       <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K4" s="18" t="s">
+      <c r="B4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1525,150 +1517,150 @@
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" s="18" t="s">
+      <c r="B5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="16"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="18"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="16"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="18"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="16"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="18"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="16"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18" t="s">
+      <c r="B10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="21" t="s">
+      <c r="B11" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="19" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1696,150 +1688,150 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" s="37" t="s">
+      <c r="A1" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="38" t="s">
+      <c r="C1" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="38" t="s">
+      <c r="D1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="38" t="s">
+      <c r="E1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
+      <c r="B2" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="18"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="16"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="16"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="18"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="16"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
+      <c r="B8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="16"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="42"/>
-      <c r="C9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="15"/>
+      <c r="F9" s="16"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="18"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="16"/>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="43" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="21"/>
+      <c r="B11" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1851,7 +1843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1862,87 +1856,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="28" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1954,7 +1948,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C470471-C426-469F-9ED6-2FEDE78EC2A1}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1964,157 +1960,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="D5" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="27" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D7" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="27" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D8" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="27" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D9" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="27" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="27" t="s">
+      <c r="D10" s="8" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="27" t="s">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2126,7 +2122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3026DB6-0F59-4D5E-A6F2-AAED52E94AFB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2137,157 +2135,157 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="B1" s="22" t="s">
+      <c r="A1" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="C2" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="27" t="s">
+      <c r="B9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="27" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="27" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D11" s="9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2300,7 +2298,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2311,58 +2309,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
+      <c r="C2" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B3" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C3" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="27" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2597,9 +2595,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98ED129A-EC5F-4310-BA42-3BB31D3FDFD8}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{98ED129A-EC5F-4310-BA42-3BB31D3FDFD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+    <ds:schemaRef ds:uri="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE7C083-BCB2-4A15-AB27-6ED599ABCFD0}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AE7C083-BCB2-4A15-AB27-6ED599ABCFD0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modifications from normal operation of codes
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\RD_WBG\osemosys_momf_RD\t3a_experiments\Experiment_1\0_From_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{010E61CC-B3D5-4AF6-8A96-9AA7324A72D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D28116-542B-4C64-8982-AA29A8B87642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -1383,16 +1383,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="D2" s="7"/>
       <c r="E2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="35" t="s">
         <v>7</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="D3" s="37"/>
       <c r="E3" s="38"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="D4" s="22"/>
       <c r="E4" s="39"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="D5" s="10"/>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="14"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>11</v>
       </c>
@@ -1477,7 +1477,7 @@
       <c r="D7" s="7"/>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -1488,7 +1488,7 @@
       <c r="D8" s="10"/>
       <c r="E8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
       <c r="E9" s="11"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="E10" s="11"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1538,22 +1538,22 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>16</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
@@ -1644,7 +1644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
@@ -1746,7 +1746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>23</v>
       </c>
@@ -1763,7 +1763,7 @@
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -1799,7 +1799,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>26</v>
       </c>
@@ -1841,12 +1841,12 @@
       <selection activeCell="A7" sqref="A7:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="12.140625" customWidth="1"/>
+    <col min="1" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>27</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>17</v>
       </c>
@@ -1882,7 +1882,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
@@ -1895,7 +1895,7 @@
       <c r="F3" s="42"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
@@ -1908,7 +1908,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="F5" s="42"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
@@ -1934,7 +1934,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
@@ -1947,7 +1947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>23</v>
       </c>
@@ -1960,7 +1960,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -1973,7 +1973,7 @@
       <c r="F9" s="42"/>
       <c r="G9" s="11"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>25</v>
       </c>
@@ -1988,7 +1988,7 @@
       <c r="F10" s="42"/>
       <c r="G10" s="11"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>26</v>
       </c>
@@ -2014,17 +2014,18 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>28</v>
       </c>
@@ -2038,7 +2039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2052,7 +2053,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>18</v>
       </c>
@@ -2066,7 +2067,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>22</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>19</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>20</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>21</v>
       </c>
@@ -2132,18 +2133,18 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>42</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>17</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>18</v>
       </c>
@@ -2185,7 +2186,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>20</v>
       </c>
@@ -2213,7 +2214,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>22</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>21</v>
       </c>
@@ -2241,7 +2242,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>23</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>24</v>
       </c>
@@ -2269,7 +2270,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>25</v>
       </c>
@@ -2283,7 +2284,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>26</v>
       </c>
@@ -2306,19 +2307,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3026DB6-0F59-4D5E-A6F2-AAED52E94AFB}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>56</v>
       </c>
@@ -2332,7 +2333,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2346,7 +2347,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>7</v>
       </c>
@@ -2360,7 +2361,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="53" t="s">
         <v>11</v>
       </c>
@@ -2416,7 +2417,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>12</v>
       </c>
@@ -2430,7 +2431,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>13</v>
       </c>
@@ -2444,7 +2445,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>14</v>
       </c>
@@ -2458,7 +2459,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>15</v>
       </c>
@@ -2481,18 +2482,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>87</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2514,7 +2515,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -2525,7 +2526,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
@@ -2536,7 +2537,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>4</v>
       </c>
@@ -2553,13 +2554,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2794,20 +2794,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2832,9 +2831,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update future 0 files. Update tourism demand sections in experiment_manager_final.py
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57D28116-542B-4C64-8982-AA29A8B87642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68226CDD-5FFB-4AAE-B6D2-E957582342DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -44,10 +44,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={617F70DF-6882-492E-802D-A1AED0ED31DC}</author>
+    <author>tc={8E173E61-7A36-4940-93D3-48588AAA0DB4}</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{617F70DF-6882-492E-802D-A1AED0ED31DC}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8E173E61-7A36-4940-93D3-48588AAA0DB4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="100">
   <si>
     <t>Techs/Demand</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Techs_Motos</t>
   </si>
   <si>
-    <t>Techs_Buses_Pri</t>
-  </si>
-  <si>
     <t>Techs_Buses_Pub</t>
   </si>
   <si>
@@ -137,12 +134,6 @@
     <t>Hybrid_D</t>
   </si>
   <si>
-    <t>PI_Hybrid_G</t>
-  </si>
-  <si>
-    <t>PI_Hybrid_D</t>
-  </si>
-  <si>
     <t>VehFuel/Fuel</t>
   </si>
   <si>
@@ -185,9 +176,6 @@
     <t>HYD</t>
   </si>
   <si>
-    <t>Hidrogeno</t>
-  </si>
-  <si>
     <t>VehFuel</t>
   </si>
   <si>
@@ -212,24 +200,6 @@
     <t>Híbrido de Diesel</t>
   </si>
   <si>
-    <t>PHG</t>
-  </si>
-  <si>
-    <t>Plug-in Hybrid Gasoline</t>
-  </si>
-  <si>
-    <t>Híbrido Enchufable de Gasolina</t>
-  </si>
-  <si>
-    <t>PHD</t>
-  </si>
-  <si>
-    <t>Plug-in Hybrid Diesel</t>
-  </si>
-  <si>
-    <t>Híbrido Enchufable de Diesel</t>
-  </si>
-  <si>
     <t>Techs</t>
   </si>
   <si>
@@ -251,33 +221,15 @@
     <t>Motocicleta</t>
   </si>
   <si>
-    <t>TRBPR</t>
-  </si>
-  <si>
-    <t>Bus Private</t>
-  </si>
-  <si>
-    <t>Autobuses privados</t>
-  </si>
-  <si>
     <t>TRBPU</t>
   </si>
   <si>
     <t>Bus Public</t>
   </si>
   <si>
-    <t>Autobuses publicos</t>
-  </si>
-  <si>
     <t>TRMBS</t>
   </si>
   <si>
-    <t>Minibus</t>
-  </si>
-  <si>
-    <t>Microbús</t>
-  </si>
-  <si>
     <t>TRXTTEL</t>
   </si>
   <si>
@@ -348,6 +300,63 @@
   </si>
   <si>
     <t>Demanda de Transporte - Carga Liviana</t>
+  </si>
+  <si>
+    <t>E6TDPASTUR</t>
+  </si>
+  <si>
+    <t>Techs_Taxi</t>
+  </si>
+  <si>
+    <t>Techs_SUV</t>
+  </si>
+  <si>
+    <t>Techs_Buses_Tur</t>
+  </si>
+  <si>
+    <t>Hidrógeno</t>
+  </si>
+  <si>
+    <t>TRTAX</t>
+  </si>
+  <si>
+    <t>Taxi Conchos</t>
+  </si>
+  <si>
+    <t>Taxis Conchos</t>
+  </si>
+  <si>
+    <t>TRSUV</t>
+  </si>
+  <si>
+    <t>Jeep</t>
+  </si>
+  <si>
+    <t>Jeeps</t>
+  </si>
+  <si>
+    <t>Autobuses públicos</t>
+  </si>
+  <si>
+    <t>TRBTUR</t>
+  </si>
+  <si>
+    <t>Bus Tourism</t>
+  </si>
+  <si>
+    <t>Bus Turístico</t>
+  </si>
+  <si>
+    <t>Minibus Guagua</t>
+  </si>
+  <si>
+    <t>Microbús Guagua</t>
+  </si>
+  <si>
+    <t>Transport Demand - Passsenger Tourism</t>
+  </si>
+  <si>
+    <t>Demanda de Transporte - Pasajero Turista</t>
   </si>
   <si>
     <t>Plain English</t>
@@ -357,7 +366,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,7 +406,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -411,7 +426,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -944,11 +959,75 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1057,29 +1136,64 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1366,7 +1480,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B2" dT="2024-02-08T19:55:57.22" personId="{54CC0947-4FCF-49EE-859B-FDDFB7B7F7AB}" id="{617F70DF-6882-492E-802D-A1AED0ED31DC}">
+  <threadedComment ref="B2" dT="2024-02-08T19:55:57.22" personId="{54CC0947-4FCF-49EE-859B-FDDFB7B7F7AB}" id="{8E173E61-7A36-4940-93D3-48588AAA0DB4}">
     <text>Correspondería a taxis</text>
   </threadedComment>
 </ThreadedComments>
@@ -1377,22 +1491,23 @@
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1402,122 +1517,157 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="44"/>
       <c r="C2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="7"/>
-      <c r="E2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="39"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="36"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="38"/>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="B8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B11" s="9"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B12" s="9"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="11"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="14" t="s">
+      <c r="B13" s="12"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1532,13 +1682,13 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
@@ -1553,274 +1703,268 @@
     <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="55" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="E1" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="H1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="I1" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="J1" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="K1" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="49" t="s">
+      <c r="L1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="M1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="33" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="58" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="48" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="K2" s="50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="B3" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="51" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="K5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="L5" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" s="63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="60"/>
+      <c r="C6" s="60"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="62"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="61"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="45"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="63"/>
+    </row>
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="K11" s="13" t="s">
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="65"/>
+      <c r="L9" s="65" t="s">
+        <v>6</v>
+      </c>
+      <c r="M9" s="66" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1835,43 +1979,43 @@
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:G7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="F1" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="27" t="s">
         <v>20</v>
-      </c>
-      <c r="F1" s="52" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="28" t="s">
         <v>6</v>
@@ -1884,7 +2028,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="10" t="s">
@@ -1897,7 +2041,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="10"/>
@@ -1910,7 +2054,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="10"/>
@@ -1923,7 +2067,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="10"/>
@@ -1936,7 +2080,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="29"/>
       <c r="C7" s="10"/>
@@ -1949,59 +2093,33 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="29"/>
       <c r="C8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="11"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="42"/>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="43"/>
-      <c r="G11" s="14"/>
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="43"/>
+      <c r="G9" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2014,113 +2132,112 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2130,13 +2247,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C470471-C426-469F-9ED6-2FEDE78EC2A1}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
@@ -2146,156 +2263,128 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D9" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2305,13 +2394,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3026DB6-0F59-4D5E-A6F2-AAED52E94AFB}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
@@ -2321,16 +2410,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -2338,139 +2427,167 @@
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="67" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" s="50" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D9" s="50" t="s">
         <v>58</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="53" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="54" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>86</v>
+      <c r="B13" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2480,13 +2597,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.109375" customWidth="1"/>
@@ -2495,13 +2612,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2509,10 +2626,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2520,32 +2637,43 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="18" t="s">
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>95</v>
+      <c r="B6" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -2554,12 +2682,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2794,25 +2923,33 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B3FEEE5-9F93-41F7-8D21-6F6305708D94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF577D57-E7AA-4634-A397-52930CDB5F6A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2831,11 +2968,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update data of the base model, with v7 model download 15/5/24 before 2pm from the drive
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IgnacioAlfaroCorrale\Desktop\RDM_RD\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68226CDD-5FFB-4AAE-B6D2-E957582342DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C78FF3-732A-4C9E-B191-2F2F21BAA50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22140" yWindow="900" windowWidth="17280" windowHeight="8880" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -1497,17 +1497,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1539,7 +1539,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
         <v>81</v>
       </c>
@@ -1551,7 +1551,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="54"/>
     </row>
-    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="35" t="s">
         <v>7</v>
       </c>
@@ -1563,7 +1563,7 @@
       <c r="E4" s="37"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>82</v>
       </c>
@@ -1575,7 +1575,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="39"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1587,7 +1587,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>83</v>
       </c>
@@ -1599,7 +1599,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
     </row>
-    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1623,7 +1623,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1635,7 +1635,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1659,7 +1659,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1688,22 +1688,22 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="M6" s="62"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1947,7 @@
       <c r="L8" s="46"/>
       <c r="M8" s="63"/>
     </row>
-    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1985,12 +1985,12 @@
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="7" width="12.109375" customWidth="1"/>
+    <col min="1" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -2026,7 +2026,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="F3" s="42"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2052,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2065,7 +2065,7 @@
       <c r="F5" s="42"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2078,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2106,7 +2106,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -2132,17 +2132,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
@@ -2156,7 +2156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
@@ -2250,18 +2250,18 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>38</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -2397,18 +2397,18 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>46</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
@@ -2436,7 +2436,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
         <v>81</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>82</v>
       </c>
@@ -2478,7 +2478,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>83</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>10</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
@@ -2600,17 +2600,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.109375" customWidth="1"/>
-    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>71</v>
       </c>
@@ -2621,7 +2621,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
@@ -2632,7 +2632,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>80</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Update the base model data. Also, clean the folder
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/4_Model/RD_Model_v7_Lucía/A1_Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C78FF3-732A-4C9E-B191-2F2F21BAA50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="106_{8D290350-7B29-4947-B92D-E4D9559AD5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89A40EBA-C802-448F-873E-6D6EA17FF947}"/>
   <bookViews>
-    <workbookView xWindow="-22140" yWindow="900" windowWidth="17280" windowHeight="8880" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -49,9 +49,9 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8E173E61-7A36-4940-93D3-48588AAA0DB4}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     Correspondería a taxis</t>
       </text>
     </comment>
@@ -143,6 +143,9 @@
     <t>Code</t>
   </si>
   <si>
+    <t>Plain_English</t>
+  </si>
+  <si>
     <t>Plain Spanish</t>
   </si>
   <si>
@@ -357,16 +360,13 @@
   </si>
   <si>
     <t>Demanda de Transporte - Pasajero Turista</t>
-  </si>
-  <si>
-    <t>Plain English</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +411,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1157,7 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,17 +1503,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1527,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1539,9 +1545,9 @@
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="52" t="s">
         <v>6</v>
@@ -1551,7 +1557,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="54"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>7</v>
       </c>
@@ -1563,9 +1569,9 @@
       <c r="E4" s="37"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="22" t="s">
@@ -1575,7 +1581,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="39"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1587,9 +1593,9 @@
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
@@ -1599,7 +1605,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1611,7 +1617,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1623,7 +1629,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1635,7 +1641,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1653,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1659,7 +1665,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1688,22 +1694,22 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
@@ -1711,16 +1717,16 @@
         <v>5</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>8</v>
@@ -1744,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1884,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1907,7 +1913,7 @@
       </c>
       <c r="M6" s="62"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1953,7 @@
       <c r="L8" s="46"/>
       <c r="M8" s="63"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1981,16 +1987,16 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="12.140625" customWidth="1"/>
+    <col min="1" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -2026,7 +2032,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2039,7 +2045,7 @@
       <c r="F3" s="42"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2058,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2065,7 +2071,7 @@
       <c r="F5" s="42"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2084,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2106,7 +2112,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -2132,17 +2138,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
@@ -2150,18 +2156,18 @@
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2170,35 +2176,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
@@ -2209,35 +2215,35 @@
         <v>18</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2250,37 +2256,37 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2289,21 +2295,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2314,77 +2320,77 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2397,197 +2403,197 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2599,81 +2605,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2682,13 +2688,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2923,15 +2928,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15197F56-C757-4BC4-834A-2FD08D72E34C}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2946,31 +2964,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF577D57-E7AA-4634-A397-52930CDB5F6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add model 0607 and generate inputs for 100 futures.
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -2697,8 +2697,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2854f1a0eb82b4299baec9a2bc5fa3aa">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e5d0997856646832757f031b0a9b789" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
     <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
     <xsd:element name="properties">
@@ -2780,7 +2780,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -2801,7 +2801,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -2820,7 +2820,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -2837,8 +2837,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2946,7 +2946,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15197F56-C757-4BC4-834A-2FD08D72E34C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A029DEC-DBF1-489A-AFBE-2A031AA24A93}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Upload again the first version of this branch
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -2697,8 +2697,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="2854f1a0eb82b4299baec9a2bc5fa3aa">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9e5d0997856646832757f031b0a9b789" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
     <xsd:import namespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
     <xsd:element name="properties">
@@ -2780,7 +2780,7 @@
         </xsd:restriction>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Etiquetas de imagen" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="20" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="71f7bd95-1200-4052-9a4e-dfdf006e181b" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -2801,7 +2801,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Compartido con" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -2820,7 +2820,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Detalles de uso compartido" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -2837,8 +2837,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de contenido"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -2946,7 +2946,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2A029DEC-DBF1-489A-AFBE-2A031AA24A93}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15197F56-C757-4BC4-834A-2FD08D72E34C}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Take the data files of the 100 futures optimal. This model is functional for tier 3, and for tier 1 is partial fuctional because the concatenate script do not make his propuose
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4507ED-B447-4389-ACB7-54B8B2B470F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA91B9-FA44-4EAE-AE3B-D82275F388CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Correct some variables in the yaml file. Also, update some data files with the functional modelo of the 100 futures in june
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA91B9-FA44-4EAE-AE3B-D82275F388CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD1BE0C-A900-4C10-A530-6E917CA35604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11235" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -1981,7 +1981,7 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
@@ -2131,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A1A324D-A0AB-4ECB-9BF7-BF12A7A5F3A8}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -2682,6 +2682,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
@@ -2691,7 +2700,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -2922,16 +2931,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2948,7 +2956,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2965,12 +2973,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update default values of the parameters into the yaml file. B1 and EM have diferents default values, specific the large value, EM has larger max value than B1. If you use the same for both you have infeasibilities
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://clgcr.sharepoint.com/sites/ClimateLeadGroup-Decarb_RD/Documentos compartidos/Decarb_RD/WBG/4_Model/RD_Model_v7_Lucía/A1_Inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD1BE0C-A900-4C10-A530-6E917CA35604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="106_{8D290350-7B29-4947-B92D-E4D9559AD5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{89A40EBA-C802-448F-873E-6D6EA17FF947}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11235" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="864" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mode_Broad" sheetId="2" r:id="rId1"/>
@@ -49,9 +49,9 @@
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{8E173E61-7A36-4940-93D3-48588AAA0DB4}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     Correspondería a taxis</t>
       </text>
     </comment>
@@ -143,6 +143,9 @@
     <t>Code</t>
   </si>
   <si>
+    <t>Plain_English</t>
+  </si>
+  <si>
     <t>Plain Spanish</t>
   </si>
   <si>
@@ -357,16 +360,13 @@
   </si>
   <si>
     <t>Demanda de Transporte - Pasajero Turista</t>
-  </si>
-  <si>
-    <t>Plain English</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,6 +411,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1157,7 +1163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1497,17 +1503,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1518,7 +1524,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -1527,7 +1533,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
@@ -1539,9 +1545,9 @@
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="51" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="52" t="s">
         <v>6</v>
@@ -1551,7 +1557,7 @@
       <c r="E3" s="53"/>
       <c r="F3" s="54"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="35" t="s">
         <v>7</v>
       </c>
@@ -1563,9 +1569,9 @@
       <c r="E4" s="37"/>
       <c r="F4" s="38"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="22" t="s">
@@ -1575,7 +1581,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="39"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
@@ -1587,9 +1593,9 @@
       <c r="E6" s="10"/>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="36"/>
       <c r="C7" s="37"/>
@@ -1599,7 +1605,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -1611,7 +1617,7 @@
       <c r="E8" s="13"/>
       <c r="F8" s="14"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="19" t="s">
         <v>10</v>
       </c>
@@ -1623,7 +1629,7 @@
       <c r="E9" s="7"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1635,7 +1641,7 @@
       <c r="E10" s="10"/>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
@@ -1647,7 +1653,7 @@
       </c>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
@@ -1659,7 +1665,7 @@
       </c>
       <c r="F12" s="11"/>
     </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
@@ -1688,22 +1694,22 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="31" t="s">
         <v>15</v>
       </c>
@@ -1711,16 +1717,16 @@
         <v>5</v>
       </c>
       <c r="C1" s="55" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="32" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G1" s="32" t="s">
         <v>8</v>
@@ -1744,7 +1750,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
@@ -1884,7 +1890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
@@ -1907,7 +1913,7 @@
       </c>
       <c r="M6" s="62"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1934,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -1947,7 +1953,7 @@
       <c r="L8" s="46"/>
       <c r="M8" s="63"/>
     </row>
-    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1981,16 +1987,16 @@
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="12.140625" customWidth="1"/>
+    <col min="1" max="7" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
@@ -2013,7 +2019,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>16</v>
       </c>
@@ -2026,7 +2032,7 @@
       <c r="F2" s="41"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2039,7 +2045,7 @@
       <c r="F3" s="42"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2052,7 +2058,7 @@
       <c r="F4" s="42"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
@@ -2065,7 +2071,7 @@
       <c r="F5" s="42"/>
       <c r="G5" s="11"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2084,7 @@
       </c>
       <c r="G6" s="11"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
@@ -2106,7 +2112,7 @@
       <c r="F8" s="42"/>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -2132,17 +2138,17 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
         <v>25</v>
       </c>
@@ -2150,18 +2156,18 @@
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2170,35 +2176,35 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>18</v>
       </c>
@@ -2209,35 +2215,35 @@
         <v>18</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2250,37 +2256,37 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>16</v>
@@ -2289,21 +2295,21 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
         <v>18</v>
       </c>
@@ -2314,77 +2320,77 @@
         <v>18</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
         <v>20</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2397,197 +2403,197 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="20" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="67" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B3" s="51" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="49" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="50" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C9" s="50" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="50" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2599,81 +2605,81 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A31B68-9A1C-4ACF-9DFA-B94C351D7F54}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.109375" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>99</v>
+        <v>27</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="17" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2691,16 +2697,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -2931,6 +2927,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>
@@ -2940,6 +2946,10 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2954,23 +2964,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update some variables to run correctly in macOS system
</commit_message>
<xml_diff>
--- a/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
+++ b/t3a_experiments/Experiment_1/0_From_Confection/A-I_Classifier_Modes_Transport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t3a_experiments\Experiment_1\0_From_Confection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys_momf\t1_confection\A1_Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E913170-C8B5-4198-9474-46D49E19196C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DA327A-0EF6-4C00-91EC-3204EB3D753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="864" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2682,16 +2682,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100CCDA0DC61E44874FB77B81A0A8C300E4" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="27b2dddd8e7dbb40e638da4098fa8bb9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c2c21c4-f980-47d5-be5b-1bb924ee96a2" xmlns:ns3="1b6bb729-2ef5-410d-b4d4-7ced22c361d1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d3d23b2622c6bf8a24212abcb0f9b2c" ns2:_="" ns3:_="">
     <xsd:import namespace="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
@@ -2922,6 +2912,16 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9c2c21c4-f980-47d5-be5b-1bb924ee96a2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2932,23 +2932,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{29396BD3-6E1D-453C-9E9B-017F5441B4C8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2967,6 +2950,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8ABA9104-BC13-491B-AC54-17D816A8EDDE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="1b6bb729-2ef5-410d-b4d4-7ced22c361d1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="9c2c21c4-f980-47d5-be5b-1bb924ee96a2"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D5A8F3-5231-46A6-A9EE-D0E0BC5EF750}">
   <ds:schemaRefs>

</xml_diff>